<commit_message>
added captions, weibull plots etc
</commit_message>
<xml_diff>
--- a/example_output/csv_data/ExtremeValues_T_return_WaveHeight.xlsx
+++ b/example_output/csv_data/ExtremeValues_T_return_WaveHeight.xlsx
@@ -423,13 +423,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>15.07332396396879</v>
+        <v>16.4</v>
       </c>
       <c r="D2">
-        <v>15.55526922371276</v>
+        <v>17.3</v>
       </c>
       <c r="E2">
-        <v>14.80232157334255</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -440,13 +440,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>15.13601698769778</v>
+        <v>17.6</v>
       </c>
       <c r="D3">
-        <v>15.71309599366206</v>
+        <v>18.7</v>
       </c>
       <c r="E3">
-        <v>14.83143896802788</v>
+        <v>16.6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -457,13 +457,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>15.26995247459638</v>
+        <v>20.2</v>
       </c>
       <c r="D4">
-        <v>16.07986381475874</v>
+        <v>22.1</v>
       </c>
       <c r="E4">
-        <v>14.87445695640271</v>
+        <v>18.7</v>
       </c>
     </row>
   </sheetData>
@@ -501,13 +501,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>14.03036310866247</v>
+        <v>15.1</v>
       </c>
       <c r="D2">
-        <v>16.59134974034517</v>
+        <v>16.1</v>
       </c>
       <c r="E2">
-        <v>12.50460781195036</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -518,13 +518,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>14.38787433298772</v>
+        <v>16.4</v>
       </c>
       <c r="D3">
-        <v>17.68611313713023</v>
+        <v>17.7</v>
       </c>
       <c r="E3">
-        <v>12.65582751527951</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -535,13 +535,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>15.19507921278876</v>
+        <v>19.4</v>
       </c>
       <c r="D4">
-        <v>20.16802466576408</v>
+        <v>21.6</v>
       </c>
       <c r="E4">
-        <v>12.91793300404705</v>
+        <v>17.8</v>
       </c>
     </row>
   </sheetData>
@@ -579,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>14.26537077374569</v>
+        <v>14.9</v>
       </c>
       <c r="D2">
-        <v>16.64903703019824</v>
+        <v>15.8</v>
       </c>
       <c r="E2">
-        <v>12.84452353697649</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -596,13 +596,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>14.63309550367449</v>
+        <v>16.3</v>
       </c>
       <c r="D3">
-        <v>17.64999476650996</v>
+        <v>17.5</v>
       </c>
       <c r="E3">
-        <v>12.98831263619856</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -613,13 +613,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>15.4183283965717</v>
+        <v>19.3</v>
       </c>
       <c r="D4">
-        <v>20.11716394495604</v>
+        <v>21.4</v>
       </c>
       <c r="E4">
-        <v>13.26398530065523</v>
+        <v>17.6</v>
       </c>
     </row>
   </sheetData>
@@ -657,13 +657,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>13.32801702167958</v>
+        <v>14.3</v>
       </c>
       <c r="D2">
-        <v>16.57203564195024</v>
+        <v>15.2</v>
       </c>
       <c r="E2">
-        <v>11.52076642528548</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -674,13 +674,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>13.79884023831141</v>
+        <v>15.5</v>
       </c>
       <c r="D3">
-        <v>17.82041312431296</v>
+        <v>16.7</v>
       </c>
       <c r="E3">
-        <v>11.73685948573129</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -691,13 +691,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>14.63707186945972</v>
+        <v>18.1</v>
       </c>
       <c r="D4">
-        <v>20.48254306212229</v>
+        <v>20.1</v>
       </c>
       <c r="E4">
-        <v>12.00354973952764</v>
+        <v>16.5</v>
       </c>
     </row>
   </sheetData>
@@ -735,13 +735,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>12.75938020822213</v>
+        <v>14.2</v>
       </c>
       <c r="D2">
-        <v>12.95861688876616</v>
+        <v>14.9</v>
       </c>
       <c r="E2">
-        <v>12.6283724428304</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -752,13 +752,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>12.78937837418965</v>
+        <v>15.2</v>
       </c>
       <c r="D3">
-        <v>13.05381149441279</v>
+        <v>16.3</v>
       </c>
       <c r="E3">
-        <v>12.64108546722015</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -769,13 +769,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>12.855149440489</v>
+        <v>17.5</v>
       </c>
       <c r="D4">
-        <v>13.25837590321734</v>
+        <v>19.3</v>
       </c>
       <c r="E4">
-        <v>12.6602465613986</v>
+        <v>16.2</v>
       </c>
     </row>
   </sheetData>
@@ -813,13 +813,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>12.30699338589113</v>
+        <v>11.2</v>
       </c>
       <c r="D2">
-        <v>15.4218520413841</v>
+        <v>11.9</v>
       </c>
       <c r="E2">
-        <v>10.40623997429353</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -830,13 +830,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>12.83025034607671</v>
+        <v>12.2</v>
       </c>
       <c r="D3">
-        <v>16.7993561516152</v>
+        <v>13.2</v>
       </c>
       <c r="E3">
-        <v>10.61414263672958</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -847,13 +847,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>13.93062488071189</v>
+        <v>14.3</v>
       </c>
       <c r="D4">
-        <v>20.1917317794382</v>
+        <v>15.8</v>
       </c>
       <c r="E4">
-        <v>10.90349211039834</v>
+        <v>13.1</v>
       </c>
     </row>
   </sheetData>
@@ -891,13 +891,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>8.689094316707964</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="D2">
-        <v>10.70933241170262</v>
+        <v>8.9</v>
       </c>
       <c r="E2">
-        <v>7.406377880321219</v>
+        <v>7.94</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -908,13 +908,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>8.962507488385986</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="D3">
-        <v>11.64175313364014</v>
+        <v>9.82</v>
       </c>
       <c r="E3">
-        <v>7.521372728371414</v>
+        <v>8.529999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -925,13 +925,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>9.597596072352754</v>
+        <v>10.7</v>
       </c>
       <c r="D4">
-        <v>13.65742668738227</v>
+        <v>11.9</v>
       </c>
       <c r="E4">
-        <v>7.664806545931145</v>
+        <v>9.82</v>
       </c>
     </row>
   </sheetData>
@@ -969,13 +969,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>7.322025078237042</v>
+        <v>7.82</v>
       </c>
       <c r="D2">
-        <v>7.764889420981837</v>
+        <v>8.26</v>
       </c>
       <c r="E2">
-        <v>7.041573490135696</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -986,13 +986,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>7.384692937438497</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="D3">
-        <v>7.956260522751805</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="E3">
-        <v>7.064137548900083</v>
+        <v>7.96</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1003,13 +1003,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>7.510215973827206</v>
+        <v>9.81</v>
       </c>
       <c r="D4">
-        <v>8.402849990422249</v>
+        <v>10.8</v>
       </c>
       <c r="E4">
-        <v>7.115425203398704</v>
+        <v>9.02</v>
       </c>
     </row>
   </sheetData>
@@ -1047,13 +1047,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>7.203291389279764</v>
+        <v>8.02</v>
       </c>
       <c r="D2">
-        <v>8.032506469448849</v>
+        <v>8.56</v>
       </c>
       <c r="E2">
-        <v>6.678017877404431</v>
+        <v>7.55</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1064,13 +1064,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>7.3157644491741</v>
+        <v>8.75</v>
       </c>
       <c r="D3">
-        <v>8.369601980417318</v>
+        <v>9.48</v>
       </c>
       <c r="E3">
-        <v>6.728833125420574</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1081,13 +1081,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>7.580567348624456</v>
+        <v>10.4</v>
       </c>
       <c r="D4">
-        <v>9.178000754055436</v>
+        <v>11.5</v>
       </c>
       <c r="E4">
-        <v>6.827716275403662</v>
+        <v>9.460000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1125,13 +1125,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>7.833819909698155</v>
+        <v>7.62</v>
       </c>
       <c r="D2">
-        <v>8.106071572619893</v>
+        <v>8.06</v>
       </c>
       <c r="E2">
-        <v>7.682558932289098</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1142,13 +1142,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>7.871419446359876</v>
+        <v>8.26</v>
       </c>
       <c r="D3">
-        <v>8.221894840817777</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="E3">
-        <v>7.695755786572456</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>7.946697406752614</v>
+        <v>9.68</v>
       </c>
       <c r="D4">
-        <v>8.483316398330704</v>
+        <v>10.7</v>
       </c>
       <c r="E4">
-        <v>7.722316040768172</v>
+        <v>8.880000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1203,13 +1203,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>6.91601624292153</v>
+        <v>7.31</v>
       </c>
       <c r="D2">
-        <v>7.535642212099806</v>
+        <v>7.78</v>
       </c>
       <c r="E2">
-        <v>6.54253178096379</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1220,13 +1220,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>6.994089039105719</v>
+        <v>7.92</v>
       </c>
       <c r="D3">
-        <v>7.771038044174509</v>
+        <v>8.56</v>
       </c>
       <c r="E3">
-        <v>6.576926793858067</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1237,13 +1237,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>7.2132363928048</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="D4">
-        <v>8.410180256354302</v>
+        <v>10.3</v>
       </c>
       <c r="E4">
-        <v>6.633462604352203</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1281,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>7.779580702890668</v>
+        <v>9.57</v>
       </c>
       <c r="D2">
-        <v>9.978320019312049</v>
+        <v>10.2</v>
       </c>
       <c r="E2">
-        <v>6.536587670914995</v>
+        <v>9.050000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1298,13 +1298,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>8.050453687953178</v>
+        <v>10.4</v>
       </c>
       <c r="D3">
-        <v>10.80511657554422</v>
+        <v>11.3</v>
       </c>
       <c r="E3">
-        <v>6.693761339441367</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1315,13 +1315,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>8.69830833339717</v>
+        <v>12.4</v>
       </c>
       <c r="D4">
-        <v>12.95200166231695</v>
+        <v>13.7</v>
       </c>
       <c r="E4">
-        <v>6.878772252994403</v>
+        <v>11.3</v>
       </c>
     </row>
   </sheetData>
@@ -1359,13 +1359,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>10.24028528846404</v>
+        <v>12.7</v>
       </c>
       <c r="D2">
-        <v>10.61479596154343</v>
+        <v>13.5</v>
       </c>
       <c r="E2">
-        <v>10.02899994577152</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1376,13 +1376,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>10.29597838772418</v>
+        <v>13.8</v>
       </c>
       <c r="D3">
-        <v>10.74383990209173</v>
+        <v>14.9</v>
       </c>
       <c r="E3">
-        <v>10.04835153825979</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1393,13 +1393,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>10.40293721199263</v>
+        <v>16.3</v>
       </c>
       <c r="D4">
-        <v>11.07406842927382</v>
+        <v>18</v>
       </c>
       <c r="E4">
-        <v>10.08559165050468</v>
+        <v>14.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>